<commit_message>
adds value ' (XaJQw) Irish - ethnic category 2001 census' to the list
</commit_message>
<xml_diff>
--- a/data/reference/ethnicity.xlsx
+++ b/data/reference/ethnicity.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_targeted_lung_health_check/mi_data/tlhc/reference/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{51BDCD49-7A3D-428C-A6E4-FD70C8735082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EED5819C-CFA3-49A9-9192-4C375E10FEA2}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{51BDCD49-7A3D-428C-A6E4-FD70C8735082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39444116-E532-4AEA-8229-82B57703A02C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="4635" windowWidth="25695" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ethnicity" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="259">
   <si>
     <t>Ethnicity</t>
   </si>
@@ -794,6 +807,9 @@
   </si>
   <si>
     <t>White:Eng/Welsh/Scot/NI/Brit -</t>
+  </si>
+  <si>
+    <t>(XaJQw) Irish - ethnic category 2001 census</t>
   </si>
 </sst>
 </file>
@@ -1338,8 +1354,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB9DDAEC-97A5-4D19-8F13-2285BABCCF92}" name="Table1" displayName="Table1" ref="A1:B257" totalsRowShown="0">
-  <autoFilter ref="A1:B257" xr:uid="{EB9DDAEC-97A5-4D19-8F13-2285BABCCF92}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB9DDAEC-97A5-4D19-8F13-2285BABCCF92}" name="Table1" displayName="Table1" ref="A1:B258" totalsRowShown="0">
+  <autoFilter ref="A1:B258" xr:uid="{EB9DDAEC-97A5-4D19-8F13-2285BABCCF92}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3E180AB1-876B-4986-8814-1FF1337475CB}" name="Ethnicity"/>
     <tableColumn id="2" xr3:uid="{D3ED0826-1607-48D9-82AF-6D6A8A9F159E}" name="EthnicGroup"/>
@@ -1645,10 +1661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B257"/>
+  <dimension ref="A1:B258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="B258" sqref="B258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3713,6 +3729,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>258</v>
+      </c>
+      <c r="B258" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
adds additional lookups for ethnicity read codes
</commit_message>
<xml_diff>
--- a/data/reference/ethnicity.xlsx
+++ b/data/reference/ethnicity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{51BDCD49-7A3D-428C-A6E4-FD70C8735082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39444116-E532-4AEA-8229-82B57703A02C}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{51BDCD49-7A3D-428C-A6E4-FD70C8735082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3F689FE-84C7-4E20-A353-FD0ED456BA6D}"/>
   <bookViews>
-    <workbookView xWindow="4635" yWindow="4635" windowWidth="25695" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6015" yWindow="510" windowWidth="12660" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ethnicity" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="297">
   <si>
     <t>Ethnicity</t>
   </si>
@@ -810,6 +810,120 @@
   </si>
   <si>
     <t>(XaJQw) Irish - ethnic category 2001 census</t>
+  </si>
+  <si>
+    <t>(9S1..)</t>
+  </si>
+  <si>
+    <t>(9S3..)</t>
+  </si>
+  <si>
+    <t>(XaFwD)</t>
+  </si>
+  <si>
+    <t>(XaFwE)</t>
+  </si>
+  <si>
+    <t>(XaFwH)</t>
+  </si>
+  <si>
+    <t>(XaFwz)</t>
+  </si>
+  <si>
+    <t>(XaFx1)</t>
+  </si>
+  <si>
+    <t>(XaIuh)</t>
+  </si>
+  <si>
+    <t>(XaJQv)</t>
+  </si>
+  <si>
+    <t>(XaJQv) British or mixed British - ethnic category</t>
+  </si>
+  <si>
+    <t>(XaJQw)</t>
+  </si>
+  <si>
+    <t>(XaJQx)</t>
+  </si>
+  <si>
+    <t>(XaJQy)</t>
+  </si>
+  <si>
+    <t>(XaJR6)</t>
+  </si>
+  <si>
+    <t>(XaJR7)</t>
+  </si>
+  <si>
+    <t>(XaJRA)</t>
+  </si>
+  <si>
+    <t>(XaJRB)</t>
+  </si>
+  <si>
+    <t>(XaJRC)</t>
+  </si>
+  <si>
+    <t>(XaJRD)</t>
+  </si>
+  <si>
+    <t>(XaJSD)</t>
+  </si>
+  <si>
+    <t>(XaJSE)</t>
+  </si>
+  <si>
+    <t>(XaJSF)</t>
+  </si>
+  <si>
+    <t>(XaJSG)</t>
+  </si>
+  <si>
+    <t>(XaJSK)</t>
+  </si>
+  <si>
+    <t>(XaJSa)</t>
+  </si>
+  <si>
+    <t>(XaQEa)</t>
+  </si>
+  <si>
+    <t>(XaR4o)</t>
+  </si>
+  <si>
+    <t>(XactH)</t>
+  </si>
+  <si>
+    <t>(XactI)</t>
+  </si>
+  <si>
+    <t>(XactK)</t>
+  </si>
+  <si>
+    <t>(Xactk)</t>
+  </si>
+  <si>
+    <t>(Xacut)</t>
+  </si>
+  <si>
+    <t>British or Mixed British</t>
+  </si>
+  <si>
+    <t>Other Asian</t>
+  </si>
+  <si>
+    <t>Other Mixed</t>
+  </si>
+  <si>
+    <t>White &amp; Asian</t>
+  </si>
+  <si>
+    <t>White &amp; Black African</t>
+  </si>
+  <si>
+    <t>White &amp; Black Caribbean</t>
   </si>
 </sst>
 </file>
@@ -1354,8 +1468,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB9DDAEC-97A5-4D19-8F13-2285BABCCF92}" name="Table1" displayName="Table1" ref="A1:B258" totalsRowShown="0">
-  <autoFilter ref="A1:B258" xr:uid="{EB9DDAEC-97A5-4D19-8F13-2285BABCCF92}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB9DDAEC-97A5-4D19-8F13-2285BABCCF92}" name="Table1" displayName="Table1" ref="A1:B296" totalsRowShown="0">
+  <autoFilter ref="A1:B296" xr:uid="{EB9DDAEC-97A5-4D19-8F13-2285BABCCF92}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{3E180AB1-876B-4986-8814-1FF1337475CB}" name="Ethnicity"/>
     <tableColumn id="2" xr3:uid="{D3ED0826-1607-48D9-82AF-6D6A8A9F159E}" name="EthnicGroup"/>
@@ -1661,10 +1775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B258"/>
+  <dimension ref="A1:B296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="B258" sqref="B258"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3737,6 +3851,310 @@
         <v>6</v>
       </c>
     </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>259</v>
+      </c>
+      <c r="B259" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>260</v>
+      </c>
+      <c r="B260" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>261</v>
+      </c>
+      <c r="B261" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>262</v>
+      </c>
+      <c r="B262" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>263</v>
+      </c>
+      <c r="B263" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>264</v>
+      </c>
+      <c r="B264" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>265</v>
+      </c>
+      <c r="B265" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>266</v>
+      </c>
+      <c r="B266" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>267</v>
+      </c>
+      <c r="B267" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>268</v>
+      </c>
+      <c r="B268" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>269</v>
+      </c>
+      <c r="B269" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>270</v>
+      </c>
+      <c r="B270" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>271</v>
+      </c>
+      <c r="B271" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>272</v>
+      </c>
+      <c r="B272" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>273</v>
+      </c>
+      <c r="B273" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>274</v>
+      </c>
+      <c r="B274" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>275</v>
+      </c>
+      <c r="B275" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>276</v>
+      </c>
+      <c r="B276" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>277</v>
+      </c>
+      <c r="B277" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>278</v>
+      </c>
+      <c r="B278" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>279</v>
+      </c>
+      <c r="B279" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>280</v>
+      </c>
+      <c r="B280" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>281</v>
+      </c>
+      <c r="B281" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>282</v>
+      </c>
+      <c r="B282" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>283</v>
+      </c>
+      <c r="B283" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>284</v>
+      </c>
+      <c r="B284" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>285</v>
+      </c>
+      <c r="B285" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>286</v>
+      </c>
+      <c r="B286" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>287</v>
+      </c>
+      <c r="B287" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>288</v>
+      </c>
+      <c r="B288" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>289</v>
+      </c>
+      <c r="B289" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>290</v>
+      </c>
+      <c r="B290" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>291</v>
+      </c>
+      <c r="B291" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>292</v>
+      </c>
+      <c r="B292" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>293</v>
+      </c>
+      <c r="B293" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>294</v>
+      </c>
+      <c r="B294" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>295</v>
+      </c>
+      <c r="B295" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>296</v>
+      </c>
+      <c r="B296" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>